<commit_message>
se agrega planificacion corregida y video demo, unificado
</commit_message>
<xml_diff>
--- a/Planificacion.xlsx
+++ b/Planificacion.xlsx
@@ -2174,9 +2174,9 @@
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
-      <c r="H19" s="21"/>
+      <c r="H19" s="19"/>
       <c r="I19" s="21"/>
-      <c r="J19" s="16"/>
+      <c r="J19" s="25"/>
     </row>
     <row r="20">
       <c r="A20" s="26" t="s">
@@ -3907,7 +3907,7 @@
         <v>152</v>
       </c>
       <c r="F17" s="38">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
       <c r="G17" s="34"/>
       <c r="H17" s="39"/>
@@ -3957,7 +3957,7 @@
         <v>152</v>
       </c>
       <c r="F19" s="38">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G19" s="34" t="s">
         <v>173</v>
@@ -9484,7 +9484,7 @@
         <v>156</v>
       </c>
       <c r="F5" s="52">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G5" s="54" t="s">
         <v>139</v>
@@ -9622,7 +9622,7 @@
         <v>215</v>
       </c>
       <c r="F11" s="52">
-        <v>0.0</v>
+        <v>0.66</v>
       </c>
       <c r="G11" s="54" t="s">
         <v>139</v>

</xml_diff>